<commit_message>
Added further formatting to improve postprocessed results
</commit_message>
<xml_diff>
--- a/results/results_pos_postprocessed.xlsx
+++ b/results/results_pos_postprocessed.xlsx
@@ -92,8 +92,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,16 +130,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD1D1D1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95C78F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79D97"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFABAFF5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFECC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -135,15 +184,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,6 +546,10 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="19" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
@@ -451,1162 +558,1162 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="8">
         <v>0.987725769524294</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="9">
         <v>0.8471126939709998</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="9">
         <v>0.8832358178580514</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="9">
         <v>0.8727423047570593</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="9">
         <v>0.9005342152124142</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="9">
         <v>0.6158738234545917</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="9">
         <v>0.6243322309844823</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="9">
         <v>0.7641821419486136</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="9">
         <v>0.6641439837191554</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="9">
         <v>0.6488170948867973</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="9">
         <v>0.5817858051386415</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="9">
         <v>0.6820783515644874</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="9">
         <v>0.7307936911727296</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="9">
         <v>0.8109895700839481</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="9">
         <v>0.2216993131518697</v>
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="9">
         <v>0.7896257221803566</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <v>0.959243908565687</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="9">
         <v>0.7351168048229089</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="9">
         <v>0.7121954282843507</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="9">
         <v>0.7321024868123587</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="9">
         <v>0.5106129113288118</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="9">
         <v>0.5568952524491334</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="9">
         <v>0.6710625470987189</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="9">
         <v>0.5913087164029138</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="9">
         <v>0.566377794523989</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="9">
         <v>0.5395001255965838</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="9">
         <v>0.6090806330067822</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="9">
         <v>0.6109645817633761</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="9">
         <v>0.7469856819894499</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="9">
         <v>0.1907189727611764</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="9">
         <v>0.9102133595081883</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="9">
         <v>0.8474453686005062</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>0.9632691016169861</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="9">
         <v>0.8764271323035594</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="9">
         <v>0.9055122178023454</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="9">
         <v>0.6520638528697629</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="9">
         <v>0.6244252725112363</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="9">
         <v>0.7937696957173116</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="9">
         <v>0.6923593532055587</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="9">
         <v>0.674278038952317</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="9">
         <v>0.6524254791548277</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="9">
         <v>0.7228392829467376</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="9">
         <v>0.7344629849666787</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="9">
         <v>0.7955778271426357</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="9">
         <v>0.2530612244897959</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="9">
         <v>0.8781086889775868</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="9">
         <v>0.8351243475591035</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="9">
         <v>0.8766502916794596</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="8">
         <v>0.9661498311329444</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="9">
         <v>0.934141848326681</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="9">
         <v>0.5964844949339884</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="9">
         <v>0.5942585201105312</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="9">
         <v>0.7942124654590114</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="9">
         <v>0.723595333128646</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="9">
         <v>0.6379336813018115</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="9">
         <v>0.605081363217685</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="9">
         <v>0.7093183911575069</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="9">
         <v>0.7448572305802886</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="9">
         <v>0.7789376727049432</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5" s="9">
         <v>0.2521492170709241</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="9">
         <v>0.9015663643858203</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="9">
         <v>0.8481863149216817</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="9">
         <v>0.897073371805441</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="9">
         <v>0.8979389942291839</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="8">
         <v>0.9737427864798022</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="9">
         <v>0.5745671887881286</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="9">
         <v>0.575886232481451</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="9">
         <v>0.7938582028029678</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="9">
         <v>0.7123248145094806</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="9">
         <v>0.6110469909315747</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="9">
         <v>0.5882934872217642</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="9">
         <v>0.6937757625721352</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="9">
         <v>0.7185078318219291</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="9">
         <v>0.7759686727122836</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="9">
         <v>0.2542456718878813</v>
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="9">
         <v>0.5632967546112538</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="9">
         <v>0.5734765351389213</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="9">
         <v>0.5161802474900771</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="9">
         <v>0.4911043660985291</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="9">
         <v>0.5483072612654681</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="8">
         <v>0.9197291618024749</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="9">
         <v>0.5116974083586271</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="9">
         <v>0.5325239318234882</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="9">
         <v>0.5218304926453421</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="9">
         <v>0.560915246322671</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="9">
         <v>0.4831660051365865</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="9">
         <v>0.5231846836329676</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="9">
         <v>0.3732430539341583</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="9">
         <v>0.5303759047396684</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="9">
         <v>0.2526266635535839</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="9">
         <v>0.5809896015074325</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="9">
         <v>0.5837113545955754</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="9">
         <v>0.5780584827971247</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="9">
         <v>0.5726847651615605</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="9">
         <v>0.5791053109079489</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="9">
         <v>0.5473515248796148</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="8">
         <v>0.8762649173005792</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="9">
         <v>0.553074185218787</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="9">
         <v>0.5753367297089818</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="9">
         <v>0.5452578686579663</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="9">
         <v>0.5157373159327239</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="9">
         <v>0.5441412520064205</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="9">
         <v>0.5433037895177611</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="9">
         <v>0.5837113545955754</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="9">
         <v>0.3210372229192807</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="9">
         <v>0.4973798539884445</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="9">
         <v>0.3743001746764008</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="9">
         <v>0.4967080216777892</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="9">
         <v>0.4460966542750929</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="9">
         <v>0.4784789716486765</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="9">
         <v>0.4917812513996506</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="9">
         <v>0.5106373449187083</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="9">
         <v>0.4135799704393783</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="9">
         <v>0.4653558471805437</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="9">
         <v>0.4546065302100596</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="9">
         <v>0.3921261253191203</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="9">
         <v>0.4082948895955569</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="9">
         <v>0.4464549648407757</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="8">
         <v>0.5760290231558203</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="9">
         <v>0.271122659259923</v>
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="9">
         <v>0.8052661488918356</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="9">
         <v>0.8569173454568416</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="9">
         <v>0.8051398623476669</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="9">
         <v>0.7606869988002778</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="9">
         <v>0.8236408410683842</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="9">
         <v>0.5466313064342995</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="9">
         <v>0.5671528698617162</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="8">
         <v>0.9720906737387132</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="9">
         <v>0.7676959020016417</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="9">
         <v>0.7023426153943297</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="9">
         <v>0.670581549535897</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="9">
         <v>0.7699690597966786</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="9">
         <v>0.6252446801793269</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="Q10" s="9">
         <v>0.794089789732904</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10" s="9">
         <v>0.266889970296404</v>
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="9">
         <v>0.6396980388939033</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="9">
         <v>0.6956593090998605</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="9">
         <v>0.6746533191105276</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="9">
         <v>0.6210306063838517</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="9">
         <v>0.6819151554935587</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="9">
         <v>0.4963485681463855</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="9">
         <v>0.5540329859686551</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="9">
         <v>0.7113317469434643</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="8">
         <v>0.9489209813735948</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="9">
         <v>0.6963157462870272</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="9">
         <v>0.6273488143103306</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="9">
         <v>0.6694838762615902</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="9">
         <v>0.5700336424058423</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11" s="9">
         <v>0.6901616476573398</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11" s="9">
         <v>0.2485025026667761</v>
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="9">
         <v>0.4682667465458494</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="9">
         <v>0.4850788182873404</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="9">
         <v>0.4443029917250159</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="9">
         <v>0.362077357996031</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="9">
         <v>0.4580821507469952</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="9">
         <v>0.4942149998127832</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="9">
         <v>0.4499943834949638</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="9">
         <v>0.4823454525030891</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="9">
         <v>0.4885610514097428</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="8">
         <v>0.9285580559403902</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="9">
         <v>0.4405586550342607</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="9">
         <v>0.5449507619725166</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="9">
         <v>0.3576964840678474</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12" s="9">
         <v>0.537724192159359</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12" s="9">
         <v>0.2425955741940315</v>
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="9">
         <v>0.581886155330439</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="9">
         <v>0.5937047756874095</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="9">
         <v>0.5972021225277376</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="9">
         <v>0.524662325132658</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="9">
         <v>0.6315123010130246</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="9">
         <v>0.5366618427399904</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="9">
         <v>0.5300289435600579</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="8">
         <v>0.6559937288953208</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="9">
         <v>0.6468282682103232</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="9">
         <v>0.5441992281717318</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="9">
         <v>0.6431500241196334</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="9">
         <v>0.6511698022190062</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="9">
         <v>0.506090207428847</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13" s="9">
         <v>0.6198142788229619</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="9">
         <v>0.4873371924746744</v>
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="9">
         <v>0.7116087486221501</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="9">
         <v>0.6696060799443059</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="9">
         <v>0.6637465916342751</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="9">
         <v>0.6416429773162383</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="9">
         <v>0.7243719904855833</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="9">
         <v>0.5104716598015896</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="9">
         <v>0.508383129314846</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="9">
         <v>0.7014561698671462</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="9">
         <v>0.6636885768985322</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="9">
         <v>0.6105470789580554</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="9">
         <v>0.571967279689041</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="8">
         <v>0.7487961942333353</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="9">
         <v>0.5887915530544758</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="9">
         <v>0.650867320299356</v>
       </c>
-      <c r="R14" s="3">
+      <c r="R14" s="9">
         <v>0.3700759993038232</v>
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="9">
         <v>0.8097441087176521</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="9">
         <v>0.7342296756782806</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="8">
         <v>0.8158161052479399</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="9">
         <v>0.777697460363356</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="9">
         <v>0.7929738325863814</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="9">
         <v>0.5289383644161727</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="9">
         <v>0.592356994843622</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="9">
         <v>0.6690761890993205</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="9">
         <v>0.6158739337863236</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="9">
         <v>0.5893209965784781</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="9">
         <v>0.535347694087032</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="9">
         <v>0.626186689798082</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="9">
         <v>0.767047371211026</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15" s="9">
         <v>0.7607826128861259</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15" s="9">
         <v>0.2688063225868633</v>
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="9">
         <v>0.5699940543040233</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="9">
         <v>0.5951641672722469</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="9">
         <v>0.6022990024443416</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="9">
         <v>0.5419171566360573</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="9">
         <v>0.5841976613595825</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="9">
         <v>0.4183127436083768</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="9">
         <v>0.4644249190724714</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="9">
         <v>0.4935588293585255</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="9">
         <v>0.4469842108740173</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="9">
         <v>0.4575543370548986</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="9">
         <v>0.4036466935324041</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="9">
         <v>0.4949461584197661</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16" s="9">
         <v>0.6269406091035211</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q16" s="8">
         <v>0.9698090770958578</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16" s="9">
         <v>0.2026161062297681</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="L21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="M21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="N21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="O21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="P21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="Q21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="R21" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2">
+      <c r="B22" s="14"/>
+      <c r="C22" s="8">
         <v>0.869878533762988</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="9">
         <v>0.8444671812630729</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="9">
         <v>0.8480190715414652</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="9">
         <v>0.8398259648935382</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="9">
         <v>0.8680726920384498</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="9">
         <v>0.5899204542750567</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="9">
         <v>0.5951595017073668</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="9">
         <v>0.7634170106053246</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="9">
         <v>0.6767464401931509</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="9">
         <v>0.6276907201192979</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22" s="9">
         <v>0.5934172520659005</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22" s="9">
         <v>0.6834184842495299</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P22" s="9">
         <v>0.7079172640610004</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22" s="9">
         <v>0.7816918849266521</v>
       </c>
-      <c r="R22" s="3">
+      <c r="R22" s="9">
         <v>0.2343748798723294</v>
       </c>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="3">
+      <c r="B23" s="14"/>
+      <c r="C23" s="9">
         <v>0.5472220700357102</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="9">
         <v>0.5104960214702992</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="9">
         <v>0.5303155839883303</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="9">
         <v>0.5032952618450608</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="9">
         <v>0.5352971812740313</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="9">
         <v>0.5195663881396327</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="9">
         <v>0.5111673766386677</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="9">
         <v>0.4997260291605512</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23" s="9">
         <v>0.5208410231782892</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23" s="9">
         <v>0.5202598817302323</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23" s="9">
         <v>0.4636764821294769</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23" s="9">
         <v>0.4918736084116483</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P23" s="9">
         <v>0.4543339360975651</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="Q23" s="8">
         <v>0.5633720941636881</v>
       </c>
-      <c r="R23" s="3">
+      <c r="R23" s="9">
         <v>0.2815955152442626</v>
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="3">
+      <c r="B24" s="14"/>
+      <c r="C24" s="9">
         <v>0.6413451676568355</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="9">
         <v>0.6601932656951516</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="9">
         <v>0.6370089774690446</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="9">
         <v>0.5820200531258114</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="8">
         <v>0.6639044877615092</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="9">
         <v>0.5168656753870097</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="9">
         <v>0.5219184624400478</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="9">
         <v>0.6377817745522552</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="9">
         <v>0.64169344963006</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M24" s="9">
         <v>0.6383511672027861</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24" s="9">
         <v>0.5776140746423823</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="9">
         <v>0.6588933750624479</v>
       </c>
-      <c r="P24" s="3">
+      <c r="P24" s="9">
         <v>0.5295713134272679</v>
       </c>
-      <c r="Q24" s="3">
+      <c r="Q24" s="9">
         <v>0.6585314457343842</v>
       </c>
-      <c r="R24" s="3">
+      <c r="R24" s="9">
         <v>0.3230802477871418</v>
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="3">
+      <c r="B25" s="14"/>
+      <c r="C25" s="9">
         <v>0.6898690815108377</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="9">
         <v>0.6646969214752637</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="9">
         <v>0.7090575538461408</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="9">
         <v>0.6598073084997067</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="9">
         <v>0.6885857469729819</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="9">
         <v>0.4736255540122747</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="9">
         <v>0.5283909569580467</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="9">
         <v>0.581317509228923</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="9">
         <v>0.5314290723301704</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M25" s="9">
         <v>0.5234376668166884</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="9">
         <v>0.469497193809718</v>
       </c>
-      <c r="O25" s="3">
+      <c r="O25" s="9">
         <v>0.5605664241089241</v>
       </c>
-      <c r="P25" s="3">
+      <c r="P25" s="9">
         <v>0.6269406091035211</v>
       </c>
-      <c r="Q25" s="2">
+      <c r="Q25" s="8">
         <v>0.7607826128861259</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25" s="9">
         <v>0.2357112144083157</v>
       </c>
     </row>
@@ -1614,84 +1721,89 @@
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="14"/>
+      <c r="C31" s="8">
         <v>0.8540526886999029</v>
       </c>
-      <c r="C31" s="3">
+      <c r="D31" s="9">
         <v>0.5925399779912117</v>
       </c>
-      <c r="D31" s="3">
+      <c r="E31" s="9">
         <v>0.6689379814466407</v>
       </c>
-      <c r="E31" s="3">
+      <c r="F31" s="9">
         <v>0.7448045744938263</v>
       </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="14"/>
+      <c r="C32" s="8">
         <v>0.5253252237226864</v>
       </c>
-      <c r="C32" s="3">
+      <c r="D32" s="9">
         <v>0.5153668823891502</v>
       </c>
-      <c r="D32" s="3">
+      <c r="E32" s="9">
         <v>0.4992754049220395</v>
       </c>
-      <c r="E32" s="3">
+      <c r="F32" s="9">
         <v>0.5088530151306265</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="14"/>
+      <c r="C33" s="8">
         <v>0.6368943903416705</v>
       </c>
-      <c r="C33" s="3">
+      <c r="D33" s="9">
         <v>0.5193920689135287</v>
       </c>
-      <c r="D33" s="3">
+      <c r="E33" s="9">
         <v>0.6308667682179863</v>
       </c>
-      <c r="E33" s="3">
+      <c r="F33" s="9">
         <v>0.594051379580826</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="14"/>
+      <c r="C34" s="9">
         <v>0.6824033224609861</v>
       </c>
-      <c r="C34" s="3">
+      <c r="D34" s="9">
         <v>0.5010082554851607</v>
       </c>
-      <c r="D34" s="3">
+      <c r="E34" s="9">
         <v>0.5332495732588848</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="8">
         <v>0.6938616109948235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated postprocessed results, added mean over others
</commit_message>
<xml_diff>
--- a/results/results_pos_postprocessed.xlsx
+++ b/results/results_pos_postprocessed.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="24">
   <si>
     <t>Group</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Introflexive</t>
+  </si>
+  <si>
+    <t>Mean over others</t>
   </si>
 </sst>
 </file>
@@ -241,10 +244,10 @@
     <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -541,13 +544,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
     <col min="2" max="19" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1447,364 +1450,490 @@
         <v>0.2026161062297681</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="1" t="s">
+    <row r="18" spans="1:18">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="9">
+        <v>0.6934031676046383</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.6814083543492481</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.6847273595120255</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.6499217519812718</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.6982054460521001</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.5371653237581533</v>
+      </c>
+      <c r="I18" s="9">
+        <v>0.5474647491378931</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.6450018040839387</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0.6125633724058003</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0.5928223748736935</v>
+      </c>
+      <c r="N18" s="9">
+        <v>0.5433975994933499</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0.6178156853535882</v>
+      </c>
+      <c r="P18" s="9">
+        <v>0.5840989503455398</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>0.6894296820487408</v>
+      </c>
+      <c r="R18" s="9">
+        <v>0.2735656408564517</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="2" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="N22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O21" s="4" t="s">
+      <c r="O22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P21" s="5" t="s">
+      <c r="P22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q21" s="5" t="s">
+      <c r="Q22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R21" s="6" t="s">
+      <c r="R22" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="1:18">
+      <c r="A23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="8">
+      <c r="B23" s="13"/>
+      <c r="C23" s="8">
         <v>0.869878533762988</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D23" s="9">
         <v>0.8444671812630729</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E23" s="9">
         <v>0.8480190715414652</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F23" s="9">
         <v>0.8398259648935382</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G23" s="9">
         <v>0.8680726920384498</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H23" s="9">
         <v>0.5899204542750567</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I23" s="9">
         <v>0.5951595017073668</v>
       </c>
-      <c r="J22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K22" s="9">
+      <c r="J23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="9">
         <v>0.7634170106053246</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L23" s="9">
         <v>0.6767464401931509</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M23" s="9">
         <v>0.6276907201192979</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N23" s="9">
         <v>0.5934172520659005</v>
       </c>
-      <c r="O22" s="9">
+      <c r="O23" s="9">
         <v>0.6834184842495299</v>
       </c>
-      <c r="P22" s="9">
+      <c r="P23" s="9">
         <v>0.7079172640610004</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="Q23" s="9">
         <v>0.7816918849266521</v>
       </c>
-      <c r="R22" s="9">
+      <c r="R23" s="9">
         <v>0.2343748798723294</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
-      <c r="A23" s="10" t="s">
+    <row r="24" spans="1:18">
+      <c r="A24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="9">
+      <c r="B24" s="13"/>
+      <c r="C24" s="9">
         <v>0.5472220700357102</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D24" s="9">
         <v>0.5104960214702992</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E24" s="9">
         <v>0.5303155839883303</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F24" s="9">
         <v>0.5032952618450608</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G24" s="9">
         <v>0.5352971812740313</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H24" s="9">
         <v>0.5195663881396327</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I24" s="9">
         <v>0.5111673766386677</v>
       </c>
-      <c r="J23" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K23" s="9">
+      <c r="J24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="9">
         <v>0.4997260291605512</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L24" s="9">
         <v>0.5208410231782892</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M24" s="9">
         <v>0.5202598817302323</v>
       </c>
-      <c r="N23" s="9">
+      <c r="N24" s="9">
         <v>0.4636764821294769</v>
       </c>
-      <c r="O23" s="9">
+      <c r="O24" s="9">
         <v>0.4918736084116483</v>
       </c>
-      <c r="P23" s="9">
+      <c r="P24" s="9">
         <v>0.4543339360975651</v>
       </c>
-      <c r="Q23" s="8">
+      <c r="Q24" s="8">
         <v>0.5633720941636881</v>
       </c>
-      <c r="R23" s="9">
+      <c r="R24" s="9">
         <v>0.2815955152442626</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
-      <c r="A24" s="11" t="s">
+    <row r="25" spans="1:18">
+      <c r="A25" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="9">
+      <c r="B25" s="13"/>
+      <c r="C25" s="9">
         <v>0.6413451676568355</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D25" s="9">
         <v>0.6601932656951516</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E25" s="9">
         <v>0.6370089774690446</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F25" s="9">
         <v>0.5820200531258114</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G25" s="8">
         <v>0.6639044877615092</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H25" s="9">
         <v>0.5168656753870097</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I25" s="9">
         <v>0.5219184624400478</v>
       </c>
-      <c r="J24" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K24" s="9">
+      <c r="J25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="9">
         <v>0.6377817745522552</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L25" s="9">
         <v>0.64169344963006</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M25" s="9">
         <v>0.6383511672027861</v>
       </c>
-      <c r="N24" s="9">
+      <c r="N25" s="9">
         <v>0.5776140746423823</v>
       </c>
-      <c r="O24" s="9">
+      <c r="O25" s="9">
         <v>0.6588933750624479</v>
       </c>
-      <c r="P24" s="9">
+      <c r="P25" s="9">
         <v>0.5295713134272679</v>
       </c>
-      <c r="Q24" s="9">
+      <c r="Q25" s="9">
         <v>0.6585314457343842</v>
       </c>
-      <c r="R24" s="9">
+      <c r="R25" s="9">
         <v>0.3230802477871418</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
-      <c r="A25" s="12" t="s">
+    <row r="26" spans="1:18">
+      <c r="A26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="9">
+      <c r="B26" s="13"/>
+      <c r="C26" s="9">
         <v>0.6898690815108377</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D26" s="9">
         <v>0.6646969214752637</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E26" s="9">
         <v>0.7090575538461408</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F26" s="9">
         <v>0.6598073084997067</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G26" s="9">
         <v>0.6885857469729819</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H26" s="9">
         <v>0.4736255540122747</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I26" s="9">
         <v>0.5283909569580467</v>
       </c>
-      <c r="J25" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25" s="9">
+      <c r="J26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="9">
         <v>0.581317509228923</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L26" s="9">
         <v>0.5314290723301704</v>
       </c>
-      <c r="M25" s="9">
+      <c r="M26" s="9">
         <v>0.5234376668166884</v>
       </c>
-      <c r="N25" s="9">
+      <c r="N26" s="9">
         <v>0.469497193809718</v>
       </c>
-      <c r="O25" s="9">
+      <c r="O26" s="9">
         <v>0.5605664241089241</v>
       </c>
-      <c r="P25" s="9">
+      <c r="P26" s="9">
         <v>0.6269406091035211</v>
       </c>
-      <c r="Q25" s="8">
+      <c r="Q26" s="8">
         <v>0.7607826128861259</v>
       </c>
-      <c r="R25" s="9">
+      <c r="R26" s="9">
         <v>0.2357112144083157</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="1" t="s">
+    <row r="28" spans="1:18">
+      <c r="A28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="9">
+        <v>0.6870787132415928</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.6699633474759469</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.6811002967112452</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0.6462371470910293</v>
+      </c>
+      <c r="G28" s="9">
+        <v>0.6889650270117431</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0.5249945179534935</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0.5391590744360322</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0.6205605808867635</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0.5926774963329177</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0.5774348589672512</v>
+      </c>
+      <c r="N28" s="9">
+        <v>0.5260512506618694</v>
+      </c>
+      <c r="O28" s="9">
+        <v>0.5986879729581376</v>
+      </c>
+      <c r="P28" s="9">
+        <v>0.5796907806723386</v>
+      </c>
+      <c r="Q28" s="8">
+        <v>0.6910945094277126</v>
+      </c>
+      <c r="R28" s="9">
+        <v>0.2686904643280124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="2" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="7" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="8">
+      <c r="B33" s="13"/>
+      <c r="C33" s="8">
         <v>0.8540526886999029</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D33" s="9">
         <v>0.5925399779912117</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E33" s="9">
         <v>0.6689379814466407</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F33" s="9">
         <v>0.7448045744938263</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="10" t="s">
+    <row r="34" spans="1:6">
+      <c r="A34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="8">
+      <c r="B34" s="13"/>
+      <c r="C34" s="8">
         <v>0.5253252237226864</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D34" s="9">
         <v>0.5153668823891502</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E34" s="9">
         <v>0.4992754049220395</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F34" s="9">
         <v>0.5088530151306265</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="11" t="s">
+    <row r="35" spans="1:6">
+      <c r="A35" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="8">
+      <c r="B35" s="13"/>
+      <c r="C35" s="8">
         <v>0.6368943903416705</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D35" s="9">
         <v>0.5193920689135287</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E35" s="9">
         <v>0.6308667682179863</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F35" s="9">
         <v>0.594051379580826</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="12" t="s">
+    <row r="36" spans="1:6">
+      <c r="A36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="9">
+      <c r="B36" s="13"/>
+      <c r="C36" s="9">
         <v>0.6824033224609861</v>
       </c>
-      <c r="D34" s="9">
+      <c r="D36" s="9">
         <v>0.5010082554851607</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E36" s="9">
         <v>0.5332495732588848</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F36" s="8">
         <v>0.6938616109948235</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="9">
+        <v>0.6148743121751145</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0.5376467674633004</v>
+      </c>
+      <c r="E38" s="9">
+        <v>0.5671543198758551</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0.6159029897350929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>